<commit_message>
fix: Integrar dados de Cachoeirinha na BASE V01_REVISADA
Corrige mapeamento de nome do município:
- Município: "Cachoeirinha" (com i)
- Arquivo PDF/JSON: "cachoerinha" (sem i)

Resultados:
- Cachoeirinha agora incluído com 83 indicadores
- Cobertura atualizada: 139/140 municípios (99.3%)
- Único município sem dados: Tocantins (consolidação estadual)

Arquivos atualizados:
- BASE_DADOS_TOCANTINS_V01_REVISADA.xlsx (139 municípios com dados)
- scripts/atualizar_base_v01_revisada.py (mapeamento corrigido)

https://claude.ai/code/session_01JtLPGJ2cBz8vSXj9imgK6Y
</commit_message>
<xml_diff>
--- a/dados/finais/BASE_DADOS_TOCANTINS_V01_REVISADA.xlsx
+++ b/dados/finais/BASE_DADOS_TOCANTINS_V01_REVISADA.xlsx
@@ -12965,115 +12965,281 @@
       <c r="AV30" t="inlineStr"/>
       <c r="AW30" t="inlineStr"/>
       <c r="AX30" t="inlineStr"/>
-      <c r="AY30" t="inlineStr"/>
-      <c r="AZ30" t="inlineStr"/>
-      <c r="BA30" t="inlineStr"/>
-      <c r="BB30" t="inlineStr"/>
+      <c r="AY30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ30" t="n">
+        <v>85</v>
+      </c>
+      <c r="BA30" t="n">
+        <v>345</v>
+      </c>
+      <c r="BB30" t="n">
+        <v>487</v>
+      </c>
       <c r="BC30" t="inlineStr"/>
       <c r="BD30" t="inlineStr"/>
       <c r="BE30" t="inlineStr"/>
       <c r="BF30" t="inlineStr"/>
       <c r="BG30" t="inlineStr"/>
-      <c r="BH30" t="inlineStr"/>
-      <c r="BI30" t="inlineStr"/>
-      <c r="BJ30" t="inlineStr"/>
-      <c r="BK30" t="inlineStr"/>
-      <c r="BL30" t="inlineStr"/>
-      <c r="BM30" t="inlineStr"/>
-      <c r="BN30" t="inlineStr"/>
-      <c r="BO30" t="inlineStr"/>
+      <c r="BH30" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI30" t="n">
+        <v>27</v>
+      </c>
+      <c r="BJ30" t="n">
+        <v>168</v>
+      </c>
+      <c r="BK30" t="n">
+        <v>203</v>
+      </c>
+      <c r="BL30" t="n">
+        <v>31</v>
+      </c>
+      <c r="BM30" t="n">
+        <v>2</v>
+      </c>
+      <c r="BN30" t="n">
+        <v>94</v>
+      </c>
+      <c r="BO30" t="n">
+        <v>69</v>
+      </c>
       <c r="BP30" t="inlineStr"/>
-      <c r="BQ30" t="inlineStr"/>
+      <c r="BQ30" t="n">
+        <v>1</v>
+      </c>
       <c r="BR30" t="inlineStr"/>
       <c r="BS30" t="inlineStr"/>
-      <c r="BT30" t="inlineStr"/>
-      <c r="BU30" t="inlineStr"/>
-      <c r="BV30" t="inlineStr"/>
-      <c r="BW30" t="inlineStr"/>
-      <c r="BX30" t="inlineStr"/>
-      <c r="BY30" t="inlineStr"/>
-      <c r="BZ30" t="inlineStr"/>
-      <c r="CA30" t="inlineStr"/>
-      <c r="CB30" t="inlineStr"/>
-      <c r="CC30" t="inlineStr"/>
-      <c r="CD30" t="inlineStr"/>
-      <c r="CE30" t="inlineStr"/>
-      <c r="CF30" t="inlineStr"/>
-      <c r="CG30" t="inlineStr"/>
-      <c r="CH30" t="inlineStr"/>
+      <c r="BT30" t="n">
+        <v>6047595</v>
+      </c>
+      <c r="BU30" t="n">
+        <v>5784934</v>
+      </c>
+      <c r="BV30" t="n">
+        <v>7694030</v>
+      </c>
+      <c r="BW30" t="n">
+        <v>9710773</v>
+      </c>
+      <c r="BX30" t="n">
+        <v>10048809</v>
+      </c>
+      <c r="BY30" t="n">
+        <v>1410954</v>
+      </c>
+      <c r="BZ30" t="n">
+        <v>1449914</v>
+      </c>
+      <c r="CA30" t="n">
+        <v>1677763</v>
+      </c>
+      <c r="CB30" t="n">
+        <v>2080034</v>
+      </c>
+      <c r="CC30" t="n">
+        <v>1993563</v>
+      </c>
+      <c r="CD30" t="n">
+        <v>2702928</v>
+      </c>
+      <c r="CE30" t="n">
+        <v>3697495</v>
+      </c>
+      <c r="CF30" t="n">
+        <v>2339247</v>
+      </c>
+      <c r="CG30" t="n">
+        <v>1955968</v>
+      </c>
+      <c r="CH30" t="n">
+        <v>5200944</v>
+      </c>
       <c r="CI30" t="inlineStr"/>
       <c r="CJ30" t="inlineStr"/>
       <c r="CK30" t="inlineStr"/>
       <c r="CL30" t="inlineStr"/>
       <c r="CM30" t="inlineStr"/>
       <c r="CN30" t="inlineStr"/>
-      <c r="CO30" t="inlineStr"/>
-      <c r="CP30" t="inlineStr"/>
-      <c r="CQ30" t="inlineStr"/>
-      <c r="CR30" t="inlineStr"/>
-      <c r="CS30" t="inlineStr"/>
-      <c r="CT30" t="inlineStr"/>
-      <c r="CU30" t="inlineStr"/>
-      <c r="CV30" t="inlineStr"/>
-      <c r="CW30" t="inlineStr"/>
-      <c r="CX30" t="inlineStr"/>
-      <c r="CY30" t="inlineStr"/>
-      <c r="CZ30" t="inlineStr"/>
-      <c r="DA30" t="inlineStr"/>
-      <c r="DB30" t="inlineStr"/>
-      <c r="DC30" t="inlineStr"/>
-      <c r="DD30" t="inlineStr"/>
-      <c r="DE30" t="inlineStr"/>
-      <c r="DF30" t="inlineStr"/>
-      <c r="DG30" t="inlineStr"/>
-      <c r="DH30" t="inlineStr"/>
-      <c r="DI30" t="inlineStr"/>
-      <c r="DJ30" t="inlineStr"/>
+      <c r="CO30" t="n">
+        <v>0.314</v>
+      </c>
+      <c r="CP30" t="n">
+        <v>0.443</v>
+      </c>
+      <c r="CQ30" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="CR30" t="n">
+        <v>0.153</v>
+      </c>
+      <c r="CS30" t="n">
+        <v>0.321</v>
+      </c>
+      <c r="CT30" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="CU30" t="n">
+        <v>0.523</v>
+      </c>
+      <c r="CV30" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="CW30" t="n">
+        <v>0.762</v>
+      </c>
+      <c r="CX30" t="n">
+        <v>0.387</v>
+      </c>
+      <c r="CY30" t="n">
+        <v>0.411</v>
+      </c>
+      <c r="CZ30" t="n">
+        <v>0.548</v>
+      </c>
+      <c r="DA30" t="n">
+        <v>40834</v>
+      </c>
+      <c r="DB30" t="n">
+        <v>45450</v>
+      </c>
+      <c r="DC30" t="n">
+        <v>56977</v>
+      </c>
+      <c r="DD30" t="n">
+        <v>64945</v>
+      </c>
+      <c r="DE30" t="n">
+        <v>59107</v>
+      </c>
+      <c r="DF30" t="n">
+        <v>3335</v>
+      </c>
+      <c r="DG30" t="n">
+        <v>4994</v>
+      </c>
+      <c r="DH30" t="n">
+        <v>3289</v>
+      </c>
+      <c r="DI30" t="n">
+        <v>2959</v>
+      </c>
+      <c r="DJ30" t="n">
+        <v>3265</v>
+      </c>
       <c r="DK30" t="inlineStr"/>
       <c r="DL30" t="inlineStr"/>
       <c r="DM30" t="inlineStr"/>
       <c r="DN30" t="inlineStr"/>
-      <c r="DO30" t="inlineStr"/>
-      <c r="DP30" t="inlineStr"/>
-      <c r="DQ30" t="inlineStr"/>
-      <c r="DR30" t="inlineStr"/>
-      <c r="DS30" t="inlineStr"/>
-      <c r="DT30" t="inlineStr"/>
-      <c r="DU30" t="inlineStr"/>
-      <c r="DV30" t="inlineStr"/>
-      <c r="DW30" t="inlineStr"/>
-      <c r="DX30" t="inlineStr"/>
+      <c r="DO30" t="n">
+        <v>11381.52</v>
+      </c>
+      <c r="DP30" t="n">
+        <v>12011.88</v>
+      </c>
+      <c r="DQ30" t="n">
+        <v>12850.16</v>
+      </c>
+      <c r="DR30" t="n">
+        <v>14685.66</v>
+      </c>
+      <c r="DS30" t="n">
+        <v>25532.91</v>
+      </c>
+      <c r="DT30" t="n">
+        <v>25904</v>
+      </c>
+      <c r="DU30" t="n">
+        <v>27219</v>
+      </c>
+      <c r="DV30" t="n">
+        <v>29234</v>
+      </c>
+      <c r="DW30" t="n">
+        <v>33542</v>
+      </c>
+      <c r="DX30" t="n">
+        <v>58547</v>
+      </c>
       <c r="DY30" t="inlineStr"/>
       <c r="DZ30" t="inlineStr"/>
       <c r="EA30" t="inlineStr"/>
       <c r="EB30" t="inlineStr"/>
-      <c r="EC30" t="inlineStr"/>
-      <c r="ED30" t="inlineStr"/>
-      <c r="EE30" t="inlineStr"/>
+      <c r="EC30" t="n">
+        <v>74.3</v>
+      </c>
+      <c r="ED30" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="EE30" t="n">
+        <v>85.3</v>
+      </c>
       <c r="EF30" t="inlineStr"/>
       <c r="EG30" t="inlineStr"/>
       <c r="EH30" t="inlineStr"/>
       <c r="EI30" t="inlineStr"/>
-      <c r="EJ30" t="inlineStr"/>
-      <c r="EK30" t="inlineStr"/>
-      <c r="EL30" t="inlineStr"/>
-      <c r="EM30" t="inlineStr"/>
-      <c r="EN30" t="inlineStr"/>
-      <c r="EO30" t="inlineStr"/>
-      <c r="EP30" t="inlineStr"/>
-      <c r="EQ30" t="inlineStr"/>
-      <c r="ER30" t="inlineStr"/>
-      <c r="ES30" t="inlineStr"/>
-      <c r="ET30" t="inlineStr"/>
-      <c r="EU30" t="inlineStr"/>
-      <c r="EV30" t="inlineStr"/>
-      <c r="EW30" t="inlineStr"/>
-      <c r="EX30" t="inlineStr"/>
-      <c r="EY30" t="inlineStr"/>
-      <c r="EZ30" t="inlineStr"/>
-      <c r="FA30" t="inlineStr"/>
-      <c r="FB30" t="inlineStr"/>
-      <c r="FC30" t="inlineStr"/>
+      <c r="EJ30" t="n">
+        <v>7476248</v>
+      </c>
+      <c r="EK30" t="n">
+        <v>7251896</v>
+      </c>
+      <c r="EL30" t="n">
+        <v>9382973</v>
+      </c>
+      <c r="EM30" t="n">
+        <v>11805995</v>
+      </c>
+      <c r="EN30" t="n">
+        <v>12048081</v>
+      </c>
+      <c r="EO30" t="n">
+        <v>3715</v>
+      </c>
+      <c r="EP30" t="n">
+        <v>3586</v>
+      </c>
+      <c r="EQ30" t="n">
+        <v>4297</v>
+      </c>
+      <c r="ER30" t="n">
+        <v>6141</v>
+      </c>
+      <c r="ES30" t="n">
+        <v>28901</v>
+      </c>
+      <c r="ET30" t="n">
+        <v>676</v>
+      </c>
+      <c r="EU30" t="n">
+        <v>661</v>
+      </c>
+      <c r="EV30" t="n">
+        <v>754</v>
+      </c>
+      <c r="EW30" t="n">
+        <v>829</v>
+      </c>
+      <c r="EX30" t="n">
+        <v>1339</v>
+      </c>
+      <c r="EY30" t="n">
+        <v>15817</v>
+      </c>
+      <c r="EZ30" t="n">
+        <v>17331</v>
+      </c>
+      <c r="FA30" t="n">
+        <v>18472</v>
+      </c>
+      <c r="FB30" t="n">
+        <v>20548</v>
+      </c>
+      <c r="FC30" t="n">
+        <v>21138</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">

</xml_diff>